<commit_message>
Added multiple Bp Patients and checked
</commit_message>
<xml_diff>
--- a/dynamo-modules/dynamo-drools/dynamo-drools-template/dynamo-drools-kjar/src/main/resources/rules/bp_rules_xls.xlsx
+++ b/dynamo-modules/dynamo-drools/dynamo-drools-template/dynamo-drools-kjar/src/main/resources/rules/bp_rules_xls.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr/>
+  <workbookPr date1904="0"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr/>
+  <calcPr refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>RuleSet</t>
   </si>
@@ -37,7 +37,7 @@
       <rPr>
         <b/>
         <sz val="12"/>
-        <color theme="7" tint="0"/>
+        <color rgb="FFFFC000"/>
         <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve">RuleTable </t>
@@ -45,7 +45,7 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color theme="7" tint="0"/>
+        <color rgb="FFFFC000"/>
         <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve">Order 
@@ -62,22 +62,53 @@
     <t>ACTION</t>
   </si>
   <si>
+    <t>lock-on-active</t>
+  </si>
+  <si>
     <t xml:space="preserve">$bpPatient:BpPatient()                                </t>
   </si>
   <si>
-    <t xml:space="preserve"> $alarms : Number(intValue ==3 )from accumulate( $t:BpPatient(),
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="64"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> $alarms : Number(intValue ==3 )from accumulate( $t:BpPatient(),
           init(Integer criticalCount= 0;), 
              action( 
-              for( int i = 0; i &lt; $bpPatient.getBpValueList().size() &amp;&amp;
+              for( int i = 0; i &lt; $t.getBpValueList().size() &amp;&amp;
                criticalCount &lt;=3; i++) {   
-               if($bpPatient.getBpValueList().get(i).getSystolic() &gt; 120 &amp;&amp; 
-                 $bpPatient.getBpValueList().get(i).getDiastolic() &gt; 80) {
-                  criticalCount++;
-                }
-               }), 
+               if($t.getBpValueList().get(i).getSystolic() &gt; 120 &amp;&amp; 
+                 $t.getBpValueList().get(i).getDiastolic() &gt; 80) {
+                criticalCount++;
+                  System.out.println();
+                  System.out.println(
+                $bpPatient.getBpValueList().get(i).getSystolic()+" "+
+                $bpPatient.getBpValueList().get(i).getDiastolic());
+                System.out.println();
+                }</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="64"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">  System.out.println( $t.getBpValueList().size() );
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="64"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">               }), 
                result(new Integer(criticalCount) )
              )
 </t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve"> System.out.println("Found Bp Patient and set warning message");
@@ -106,22 +137,25 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <name val="Calibri"/>
-      <color theme="1"/>
+      <color indexed="64"/>
       <sz val="11.000000"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.000000"/>
     </font>
     <font>
       <name val="Arial"/>
       <b/>
-      <color theme="1" tint="0"/>
+      <color indexed="64"/>
       <sz val="12.000000"/>
     </font>
     <font>
       <name val="Arial"/>
-      <color theme="1" tint="0"/>
+      <color indexed="64"/>
       <sz val="12.000000"/>
     </font>
     <font>
@@ -136,18 +170,8 @@
     </font>
     <font>
       <name val="Arial"/>
-      <color theme="1" tint="0"/>
-      <sz val="10.000000"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <color theme="1"/>
-      <sz val="10.000000"/>
-    </font>
-    <font>
-      <name val="Arial"/>
       <b/>
-      <color theme="7" tint="0"/>
+      <color rgb="FFFFC000"/>
       <sz val="12.000000"/>
     </font>
     <font>
@@ -159,18 +183,18 @@
     <font>
       <name val="Arial"/>
       <b/>
-      <color theme="7" tint="0"/>
+      <color rgb="FFFFC000"/>
       <sz val="10.000000"/>
     </font>
     <font>
       <name val="Arial"/>
       <b/>
-      <color theme="7" tint="0"/>
+      <color rgb="FFFFC000"/>
       <sz val="11.000000"/>
     </font>
     <font>
       <name val="Arial"/>
-      <color theme="7" tint="0"/>
+      <color rgb="FFFFC000"/>
       <sz val="10.000000"/>
     </font>
   </fonts>
@@ -183,14 +207,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="0"/>
-        <bgColor theme="0" tint="0"/>
+        <fgColor indexed="65"/>
+        <bgColor indexed="26"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0"/>
-        <bgColor theme="4" tint="0"/>
+        <fgColor rgb="FF5B9BD5"/>
+        <bgColor indexed="55"/>
       </patternFill>
     </fill>
     <fill>
@@ -210,29 +234,29 @@
     </border>
     <border>
       <left style="hair">
-        <color indexed="64"/>
+        <color theme="1"/>
       </left>
       <right style="hair">
-        <color indexed="64"/>
+        <color theme="1"/>
       </right>
       <top style="hair">
-        <color indexed="64"/>
+        <color theme="1"/>
       </top>
       <bottom style="hair">
-        <color indexed="64"/>
+        <color theme="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="hair">
-        <color indexed="64"/>
+        <color theme="1"/>
       </left>
       <right/>
       <top style="hair">
-        <color indexed="64"/>
+        <color theme="1"/>
       </top>
       <bottom style="hair">
-        <color indexed="64"/>
+        <color theme="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -240,32 +264,32 @@
       <left/>
       <right/>
       <top style="hair">
-        <color indexed="64"/>
+        <color theme="1"/>
       </top>
       <bottom style="hair">
-        <color indexed="64"/>
+        <color theme="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="hair">
-        <color indexed="64"/>
+        <color theme="1"/>
       </right>
       <top style="hair">
-        <color indexed="64"/>
+        <color theme="1"/>
       </top>
       <bottom style="hair">
-        <color indexed="64"/>
+        <color theme="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="hair">
-        <color indexed="64"/>
+        <color theme="1"/>
       </left>
       <right style="hair">
-        <color indexed="64"/>
+        <color theme="1"/>
       </right>
       <top/>
       <bottom/>
@@ -273,140 +297,133 @@
     </border>
     <border>
       <left style="hair">
-        <color indexed="64"/>
+        <color theme="1"/>
       </left>
       <right style="hair">
-        <color indexed="64"/>
+        <color theme="1"/>
       </right>
       <top/>
       <bottom style="hair">
-        <color indexed="64"/>
+        <color theme="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="6">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="36">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="1" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf fontId="2" fillId="2" borderId="2" numFmtId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf fontId="2" fillId="2" borderId="3" numFmtId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf fontId="2" fillId="2" borderId="4" numFmtId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf fontId="2" fillId="2" borderId="1" numFmtId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="2" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf fontId="3" fillId="2" borderId="2" numFmtId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf fontId="3" fillId="2" borderId="3" numFmtId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf fontId="3" fillId="2" borderId="4" numFmtId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf fontId="3" fillId="2" borderId="1" numFmtId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="3" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="4" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="4" fillId="0" borderId="2" numFmtId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf fontId="4" fillId="0" borderId="3" numFmtId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf fontId="4" fillId="0" borderId="4" numFmtId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="0" borderId="2" numFmtId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf fontId="5" fillId="0" borderId="3" numFmtId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf fontId="5" fillId="0" borderId="4" numFmtId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf fontId="5" fillId="0" borderId="1" numFmtId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="3" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf fontId="6" fillId="0" borderId="2" numFmtId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf fontId="6" fillId="0" borderId="3" numFmtId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf fontId="6" fillId="0" borderId="4" numFmtId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf fontId="6" fillId="0" borderId="1" numFmtId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="4" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf fontId="5" fillId="0" borderId="1" numFmtId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf fontId="6" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf fontId="7" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf fontId="8" fillId="3" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf fontId="8" fillId="3" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf fontId="8" fillId="3" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf fontId="8" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf fontId="9" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf fontId="9" fillId="3" borderId="1" numFmtId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf fontId="10" fillId="3" borderId="1" numFmtId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="8" fillId="3" borderId="1" numFmtId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf fontId="9" fillId="3" borderId="1" numFmtId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf fontId="6" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf fontId="6" fillId="0" borderId="2" numFmtId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="8" fillId="3" borderId="1" numFmtId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf fontId="8" fillId="3" borderId="1" numFmtId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="5" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf fontId="5" fillId="0" borderId="2" numFmtId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf fontId="6" fillId="0" borderId="4" numFmtId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="0" borderId="4" numFmtId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="6" fillId="0" borderId="1" numFmtId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf fontId="6" fillId="0" borderId="1" numFmtId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="6" fillId="0" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf fontId="11" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="0" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf fontId="5" fillId="0" borderId="1" numFmtId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf fontId="10" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="11" fillId="4" borderId="1" numFmtId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="10" fillId="4" borderId="1" numFmtId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="11" fillId="4" borderId="6" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="11" fillId="4" borderId="1" numFmtId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="10" fillId="4" borderId="6" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="10" fillId="4" borderId="1" numFmtId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="6" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf fontId="6" fillId="0" borderId="1" numFmtId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="0" borderId="1" numFmtId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf fontId="6" fillId="0" borderId="1" numFmtId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="0" borderId="1" numFmtId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf fontId="6" fillId="0" borderId="1" numFmtId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="0" borderId="1" numFmtId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf fontId="6" fillId="0" borderId="1" numFmtId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="0" borderId="1" numFmtId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
+    <cellStyle name="Currency" xfId="3" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -702,47 +719,47 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="">
       <a:majorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface="Arial"/>
@@ -754,85 +771,32 @@
         <a:cs typeface="Arial"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
+        <a:solidFill/>
+        <a:solidFill/>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+        <a:ln w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -869,38 +833,11 @@
           <a:schemeClr val="phClr"/>
         </a:solidFill>
         <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
+          <a:srgbClr val="000000"/>
         </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
+        <a:solidFill>
+          <a:srgbClr val="000000"/>
+        </a:solidFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
@@ -910,18 +847,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetPr filterMode="0">
+    <outlinePr applyStyles="0" showOutlineSymbols="1" summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
+  </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100">
-      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showGridLines="1" showRowColHeaders="1" workbookViewId="0" zoomScale="100">
+      <selection activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.25"/>
   <cols>
-    <col bestFit="1" customWidth="1" min="1" max="1" width="20.57421875"/>
-    <col bestFit="1" customWidth="1" min="2" max="2" width="46.140625"/>
-    <col bestFit="1" customWidth="1" min="3" max="3" width="85.140625"/>
-    <col bestFit="1" customWidth="1" min="4" max="4" width="39.7109375"/>
-    <col bestFit="1" customWidth="1" min="5" max="5" width="59.00390625"/>
+    <col bestFit="1" customWidth="1" min="1" max="1" style="0" width="20.57"/>
+    <col bestFit="1" customWidth="1" min="2" max="2" style="0" width="46.140000000000001"/>
+    <col bestFit="1" customWidth="1" min="3" max="3" style="0" width="85.129999999999995"/>
+    <col bestFit="1" customWidth="1" min="4" max="4" style="0" width="39.700000000000003"/>
+    <col bestFit="1" customWidth="1" min="5" max="5" style="0" width="59.009999999999998"/>
   </cols>
   <sheetData>
     <row r="1" ht="15">
@@ -946,132 +887,136 @@
       <c r="D2" s="9"/>
       <c r="E2" s="10"/>
     </row>
-    <row r="3" ht="14.25">
+    <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="11" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="15"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
     </row>
     <row r="4" ht="30">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="20"/>
-    </row>
-    <row r="5" ht="14.25">
-      <c r="A5" s="21" t="s">
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+    </row>
+    <row r="5" ht="14.15">
+      <c r="A5" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="24"/>
-    </row>
-    <row r="6" ht="191.25">
-      <c r="A6" s="25"/>
-      <c r="B6" s="26" t="s">
+      <c r="E5" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="27" t="s">
+    </row>
+    <row r="6" ht="255">
+      <c r="A6" s="20"/>
+      <c r="B6" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="28"/>
-      <c r="E6" s="29"/>
+      <c r="C6" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="23"/>
+      <c r="E6" s="24" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" ht="38.25">
-      <c r="A7" s="25"/>
-      <c r="B7" s="30"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="29"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="26"/>
     </row>
     <row r="8" ht="14.25">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="34" t="s">
+      <c r="B8" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="35" t="s">
+      <c r="C8" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="35"/>
+      <c r="D8" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="30"/>
     </row>
     <row r="9" ht="25.5">
-      <c r="A9" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="36">
+      <c r="A9" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="31">
         <v>5000</v>
       </c>
-      <c r="C9" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="36" t="s">
+      <c r="C9" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="37"/>
+      <c r="D9" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="32"/>
     </row>
     <row r="10" ht="14.25">
-      <c r="A10" s="36"/>
-      <c r="B10" s="38"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="39"/>
+      <c r="A10" s="31"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="34"/>
     </row>
     <row r="11" ht="14.25">
-      <c r="A11" s="36"/>
-      <c r="B11" s="40"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
+      <c r="A11" s="31"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
     </row>
     <row r="12" ht="14.25">
-      <c r="A12" s="36"/>
-      <c r="B12" s="40"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
+      <c r="A12" s="31"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
     </row>
     <row r="13" ht="14.25">
-      <c r="A13" s="36"/>
-      <c r="B13" s="40"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
+      <c r="A13" s="31"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
     </row>
     <row r="14" ht="14.25">
-      <c r="A14" s="36"/>
-      <c r="B14" s="40"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
+      <c r="A14" s="31"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
     </row>
     <row r="15" ht="14.25">
-      <c r="A15" s="36"/>
-      <c r="B15" s="40"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
+      <c r="A15" s="31"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1079,8 +1024,8 @@
     <mergeCell ref="B4:D4"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="-1" fitToHeight="1" fitToWidth="1" horizontalDpi="600" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="600"/>
+  <pageMargins left="0.70069444444444395" right="0.70069444444444395" top="0.75208333333333299" bottom="0.75208333333333299" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="300"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>